<commit_message>
Se agrega Network devices al reporte
</commit_message>
<xml_diff>
--- a/src/Reporte_Discovery.xlsx
+++ b/src/Reporte_Discovery.xlsx
@@ -1,31 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jesusarellano/Documents/AXONIUS/Desarrollo/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2343E8A4-0DF1-3541-933F-231F2DC27EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8CDCA54-B89A-034A-9CAF-AD2B78FE782C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17160" activeTab="3" xr2:uid="{F6E7C25F-76F7-4D4B-8233-292C3B48EDEA}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17160" xr2:uid="{F6E7C25F-76F7-4D4B-8233-292C3B48EDEA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Resumen -" sheetId="1" r:id="rId1"/>
+    <sheet name="Resumen" sheetId="1" r:id="rId1"/>
     <sheet name="No Identificados" sheetId="6" r:id="rId2"/>
     <sheet name="Identificados (OTROS)" sheetId="5" r:id="rId3"/>
     <sheet name="Inventario - PC" sheetId="4" r:id="rId4"/>
-    <sheet name="Inventario -" sheetId="2" r:id="rId5"/>
-    <sheet name="Inventario - EOL" sheetId="7" r:id="rId6"/>
-    <sheet name="MAC Address -" sheetId="3" r:id="rId7"/>
+    <sheet name="Inventario - Red" sheetId="8" r:id="rId5"/>
+    <sheet name="Inventario" sheetId="2" r:id="rId6"/>
+    <sheet name="Inventario - EOL" sheetId="7" r:id="rId7"/>
+    <sheet name="MAC Address" sheetId="3" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Inventario -'!$A$5:$J$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Inventario - EOL'!$A$2:$H$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Inventario!$A$5:$J$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Inventario - EOL'!$A$2:$H$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Inventario - PC'!$A$5:$G$2261</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'MAC Address -'!$A$1:$C$92</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'MAC Address'!$A$1:$C$92</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -431,9 +432,6 @@
     <t xml:space="preserve">PCs CARSO - Inventario </t>
   </si>
   <si>
-    <t>Dispositivos No Identificados</t>
-  </si>
-  <si>
     <t>NETWORK</t>
   </si>
   <si>
@@ -537,9 +535,6 @@
   </si>
   <si>
     <t>00:0C:29:F7:DE:D7</t>
-  </si>
-  <si>
-    <t>Otros dispositivos identificados</t>
   </si>
   <si>
     <t>Virtual Patching</t>
@@ -562,6 +557,12 @@
   </si>
   <si>
     <t>Linux Red Hat 7.9</t>
+  </si>
+  <si>
+    <t>Otros dispositivos identificados (No servidores)</t>
+  </si>
+  <si>
+    <t>Dispositivos No Identificados (Servidores)</t>
   </si>
 </sst>
 </file>
@@ -876,7 +877,7 @@
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -949,9 +950,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="9" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1059,11 +1057,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
@@ -1454,97 +1452,97 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64B986C9-0500-584C-A3B3-4FE9460B9C9D}">
   <dimension ref="A2:E20"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="200" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="53"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="52"/>
       <c r="E3" s="19">
         <v>7507</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="65"/>
-      <c r="B4" s="54" t="s">
-        <v>142</v>
-      </c>
-      <c r="C4" s="55"/>
-      <c r="D4" s="56"/>
+      <c r="A4" s="64"/>
+      <c r="B4" s="53" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="54"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="38">
         <f>E5+E9+E12+E13</f>
         <v>4109</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="66"/>
-      <c r="B5" s="68"/>
-      <c r="C5" s="57" t="s">
+      <c r="A5" s="65"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="58"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="39">
-        <f>COUNTA('Inventario -'!B6:B1048576)</f>
+        <f>COUNTA(Inventario!B6:B1048576)</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="66"/>
-      <c r="B6" s="69"/>
-      <c r="C6" s="59"/>
+      <c r="A6" s="65"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="58"/>
       <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="42" t="e">
-        <f>COUNTIF('Inventario -'!#REF!,"SINO")+COUNTIF('Inventario -'!#REF!,"SISI")</f>
+      <c r="E6" s="41" t="e">
+        <f>COUNTIF(Inventario!#REF!,"SINO")+COUNTIF(Inventario!#REF!,"SISI")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="66"/>
-      <c r="B7" s="69"/>
-      <c r="C7" s="60"/>
+      <c r="A7" s="65"/>
+      <c r="B7" s="68"/>
+      <c r="C7" s="59"/>
       <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="42" t="e">
-        <f>COUNTIF('Inventario -'!#REF!,"NOSI")</f>
+      <c r="E7" s="41" t="e">
+        <f>COUNTIF(Inventario!#REF!,"NOSI")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="66"/>
-      <c r="B8" s="69"/>
-      <c r="C8" s="61"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="60"/>
       <c r="D8" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="E8" s="42" t="e">
-        <f>COUNTIF('Inventario -'!#REF!,"NONO")</f>
+      <c r="E8" s="41" t="e">
+        <f>COUNTIF(Inventario!#REF!,"NONO")</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="66"/>
-      <c r="B9" s="69"/>
+      <c r="A9" s="65"/>
+      <c r="B9" s="68"/>
       <c r="C9" s="12"/>
       <c r="D9" s="13" t="s">
         <v>8</v>
@@ -1555,46 +1553,46 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="66"/>
-      <c r="B10" s="69"/>
-      <c r="C10" s="63"/>
+      <c r="A10" s="65"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="62"/>
       <c r="D10" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="E10" s="42">
+      <c r="E10" s="41">
         <f>COUNTIF('Inventario - PC'!F6:F1048576,"SI")</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="66"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="64"/>
+      <c r="A11" s="65"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="63"/>
       <c r="D11" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E11" s="42">
+      <c r="E11" s="41">
         <f>COUNTIF('Inventario - PC'!F6:F1048576,"no")</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="66"/>
-      <c r="B12" s="69"/>
+      <c r="A12" s="65"/>
+      <c r="B12" s="68"/>
       <c r="C12" s="14"/>
       <c r="D12" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="E12" s="40">
+        <v>143</v>
+      </c>
+      <c r="E12" s="39">
         <v>3726</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="66"/>
-      <c r="B13" s="70"/>
+      <c r="A13" s="65"/>
+      <c r="B13" s="69"/>
       <c r="C13" s="14"/>
       <c r="D13" s="16" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="E13" s="39">
         <f>28+5+2+238+108</f>
@@ -1602,13 +1600,13 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="67"/>
-      <c r="B14" s="62" t="s">
-        <v>127</v>
-      </c>
-      <c r="C14" s="62"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="41">
+      <c r="A14" s="66"/>
+      <c r="B14" s="61" t="s">
+        <v>170</v>
+      </c>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="40">
         <f>E3-E4</f>
         <v>3398</v>
       </c>
@@ -1620,39 +1618,39 @@
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="47" t="s">
+      <c r="A18" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="48"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="49"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="48"/>
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
       <c r="E20" s="5"/>
     </row>
   </sheetData>
@@ -1674,11 +1672,12 @@
   <hyperlinks>
     <hyperlink ref="E14" location="'No Identificados'!A1" display="'No Identificados'!A1" xr:uid="{6BB12730-5417-6B47-A10E-4E1A3D79A481}"/>
     <hyperlink ref="E13" location="'Identificados (OTROS)'!A1" display="'Identificados (OTROS)'!A1" xr:uid="{50A36349-ACA9-9D4F-91F0-3334063128F8}"/>
-    <hyperlink ref="E9" location="'Inventario - PC CARSO'!A1" display="'Inventario - PC CARSO'!A1" xr:uid="{0DFC20D2-EC8C-E747-B690-87E905C24920}"/>
-    <hyperlink ref="E5" location="'Inventario - CARSO'!A1" display="'Inventario - CARSO'!A1" xr:uid="{AC498F9B-A70A-FC46-8C40-0AF85EBD504E}"/>
+    <hyperlink ref="E9" location="'Inventario - PC'!A1" display="'Inventario - PC'!A1" xr:uid="{0DFC20D2-EC8C-E747-B690-87E905C24920}"/>
+    <hyperlink ref="E5" location="Inventario!A1" display="Inventario!A1" xr:uid="{AC498F9B-A70A-FC46-8C40-0AF85EBD504E}"/>
     <hyperlink ref="E10" location="'Inventario - PC CARSO'!A1" display="'Inventario - PC CARSO'!A1" xr:uid="{C3DB093C-FD53-8345-893E-54AE37D247D8}"/>
     <hyperlink ref="E11" location="'Inventario - PC CARSO'!A1" display="'Inventario - PC CARSO'!A1" xr:uid="{3F18461C-E759-7D45-A6FA-468FBD08CA6A}"/>
     <hyperlink ref="E6:E8" location="'Inventario - CARSO'!A1" display="'Inventario - CARSO'!A1" xr:uid="{DBCEC83B-70F1-E743-8639-7801983E782E}"/>
+    <hyperlink ref="E12" location="'Inventario - Red'!A1" display="'Inventario - Red'!A1" xr:uid="{CBA6A172-1EA2-E44C-99A0-76417203F0C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1688,9 +1687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD622630-D4FA-2845-9496-22A7F9923B0A}">
   <dimension ref="A2:B10"/>
   <sheetViews>
-    <sheetView zoomScale="333" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
+    <sheetView zoomScale="333" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1705,22 +1702,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="71" t="s">
-        <v>146</v>
-      </c>
-      <c r="B2" s="71"/>
+      <c r="A2" s="70" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="70"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="33" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="33" t="s">
         <v>147</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B4" s="36">
         <v>15</v>
@@ -1728,7 +1725,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B5" s="36">
         <v>8</v>
@@ -1736,7 +1733,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B6" s="36">
         <v>9</v>
@@ -1744,7 +1741,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B7" s="36">
         <v>6</v>
@@ -1752,7 +1749,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B8" s="36">
         <v>265</v>
@@ -1760,7 +1757,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B9" s="36">
         <v>137</v>
@@ -1768,7 +1765,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B10" s="37"/>
     </row>
@@ -1785,7 +1782,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView zoomScale="253" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1794,26 +1791,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="72"/>
-      <c r="B1" s="72"/>
+      <c r="A1" s="71"/>
+      <c r="B1" s="71"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="71" t="s">
-        <v>149</v>
-      </c>
-      <c r="B2" s="71"/>
+      <c r="A2" s="70" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="70"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="33" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="33" t="s">
         <v>147</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B4" s="36">
         <v>28</v>
@@ -1821,7 +1818,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B5" s="36">
         <v>5</v>
@@ -1829,7 +1826,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B6" s="36">
         <v>2</v>
@@ -1837,7 +1834,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B7" s="36">
         <v>237</v>
@@ -1871,7 +1868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D99573C-41DA-9946-A7D2-72A90E8026DF}">
   <dimension ref="A3:G2262"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
+    <sheetView zoomScale="134" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:G3"/>
     </sheetView>
   </sheetViews>
@@ -1887,47 +1884,47 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="72" t="s">
         <v>126</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
     </row>
     <row r="4" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="74" t="s">
+      <c r="A4" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="74" t="s">
+      <c r="C4" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="74" t="s">
-        <v>151</v>
-      </c>
-      <c r="E4" s="74" t="s">
+      <c r="D4" s="73" t="s">
+        <v>150</v>
+      </c>
+      <c r="E4" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="74" t="s">
+      <c r="F4" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="74" t="s">
-        <v>164</v>
+      <c r="G4" s="73" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="75"/>
-      <c r="B5" s="75"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
+      <c r="A5" s="74"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -1940,7 +1937,7 @@
         <v>124</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>125</v>
@@ -10999,6 +10996,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1672578-C142-3147-975F-F4C18817BC09}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FCF3923-7F5F-D04D-BC83-E515520DDC80}">
   <dimension ref="A3:J6"/>
   <sheetViews>
@@ -11006,7 +11017,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11022,64 +11033,64 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:10" ht="24" x14ac:dyDescent="0.3">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="74" t="s">
-        <v>151</v>
-      </c>
-      <c r="E4" s="77" t="s">
+      <c r="D4" s="73" t="s">
+        <v>150</v>
+      </c>
+      <c r="E4" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="77" t="s">
+      <c r="F4" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="77" t="s">
+      <c r="G4" s="75" t="s">
         <v>15</v>
       </c>
       <c r="H4" s="76" t="s">
         <v>120</v>
       </c>
       <c r="I4" s="76"/>
-      <c r="J4" s="77" t="s">
+      <c r="J4" s="75" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="77"/>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
+      <c r="A5" s="75"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
       <c r="H5" s="2" t="s">
         <v>121</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="J5" s="77"/>
+      <c r="J5" s="75"/>
     </row>
     <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -11092,7 +11103,7 @@
         <v>23</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>19</v>
@@ -11139,7 +11150,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0C24AD6-1BF5-5642-97BB-C604A24EBCAD}">
   <dimension ref="A1:K4"/>
   <sheetViews>
@@ -11150,81 +11161,81 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.5" style="44" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="20.33203125" style="45" customWidth="1"/>
+    <col min="2" max="2" width="40.5" style="43" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="20.33203125" style="44" customWidth="1"/>
     <col min="6" max="7" width="10.83203125" style="10"/>
     <col min="8" max="8" width="17.33203125" style="10" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="78" t="s">
-        <v>165</v>
-      </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
+      <c r="A1" s="77" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="77" t="s">
+      <c r="C2" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="74" t="s">
-        <v>151</v>
-      </c>
-      <c r="E2" s="74" t="s">
-        <v>169</v>
-      </c>
-      <c r="F2" s="79" t="s">
+      <c r="D2" s="73" t="s">
+        <v>150</v>
+      </c>
+      <c r="E2" s="73" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="74" t="s">
+      <c r="G2" s="73" t="s">
+        <v>162</v>
+      </c>
+      <c r="H2" s="78" t="s">
         <v>164</v>
       </c>
-      <c r="H2" s="79" t="s">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="78"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="78"/>
+    </row>
+    <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="42">
+        <v>1</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" s="45" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="79"/>
-      <c r="B3" s="80"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="79"/>
-    </row>
-    <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="43">
-        <v>1</v>
-      </c>
-      <c r="B4" s="43" t="s">
-        <v>167</v>
-      </c>
-      <c r="C4" s="46" t="s">
+      <c r="D4" s="45"/>
+      <c r="E4" s="45" t="s">
         <v>168</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46" t="s">
-        <v>170</v>
-      </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43">
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42">
         <v>10</v>
       </c>
     </row>
@@ -11245,7 +11256,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24104E5D-E9BE-1C47-A585-F1F6E5A14A55}">
   <dimension ref="A1:K101"/>
   <sheetViews>
@@ -11270,10 +11281,10 @@
         <v>116</v>
       </c>
       <c r="J1" t="s">
+        <v>151</v>
+      </c>
+      <c r="K1" t="s">
         <v>152</v>
-      </c>
-      <c r="K1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -12035,7 +12046,7 @@
         <v>2</v>
       </c>
       <c r="J52" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K52">
         <v>2</v>
@@ -12080,7 +12091,7 @@
         <v>#N/A</v>
       </c>
       <c r="J55" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K55">
         <v>1</v>
@@ -12125,7 +12136,7 @@
         <v>1</v>
       </c>
       <c r="C58" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J58" t="s">
         <v>79</v>
@@ -12218,7 +12229,7 @@
         <v>#N/A</v>
       </c>
       <c r="J64" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K64">
         <v>1</v>
@@ -12308,7 +12319,7 @@
         <v>3676</v>
       </c>
       <c r="C70" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J70" t="s">
         <v>91</v>
@@ -12326,7 +12337,7 @@
         <v>5</v>
       </c>
       <c r="C71" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J71" t="s">
         <v>68</v>
@@ -12344,7 +12355,7 @@
         <v>4</v>
       </c>
       <c r="C72" s="35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J72" t="s">
         <v>93</v>
@@ -12362,7 +12373,7 @@
         <v>2</v>
       </c>
       <c r="C73" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J73" t="s">
         <v>94</v>
@@ -12380,10 +12391,10 @@
         <v>1</v>
       </c>
       <c r="C74" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J74" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K74">
         <v>1</v>
@@ -12398,7 +12409,7 @@
         <v>1</v>
       </c>
       <c r="C75" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J75" t="s">
         <v>73</v>
@@ -12416,10 +12427,10 @@
         <v>237</v>
       </c>
       <c r="C76" s="24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J76" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K76">
         <v>1</v>
@@ -12434,7 +12445,7 @@
         <v>27</v>
       </c>
       <c r="C77" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J77" t="s">
         <v>98</v>
@@ -12452,7 +12463,7 @@
         <v>2</v>
       </c>
       <c r="C78" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J78" t="s">
         <v>100</v>
@@ -12470,10 +12481,10 @@
         <v>19</v>
       </c>
       <c r="C79" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J79" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K79">
         <v>1</v>
@@ -12488,7 +12499,7 @@
         <v>3</v>
       </c>
       <c r="C80" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J80" t="s">
         <v>101</v>
@@ -12506,7 +12517,7 @@
         <v>2</v>
       </c>
       <c r="C81" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J81" t="s">
         <v>102</v>
@@ -12524,7 +12535,7 @@
         <v>4</v>
       </c>
       <c r="C82" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J82" t="s">
         <v>74</v>
@@ -12542,10 +12553,10 @@
         <v>1</v>
       </c>
       <c r="C83" s="32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J83" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K83">
         <v>1</v>
@@ -12560,7 +12571,7 @@
         <v>1</v>
       </c>
       <c r="C84" s="32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J84" t="s">
         <v>103</v>
@@ -12578,7 +12589,7 @@
         <v>15</v>
       </c>
       <c r="C85" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J85" t="s">
         <v>104</v>
@@ -12596,7 +12607,7 @@
         <v>8</v>
       </c>
       <c r="C86" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J86" t="s">
         <v>105</v>
@@ -12614,7 +12625,7 @@
         <v>9</v>
       </c>
       <c r="C87" s="26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J87" t="s">
         <v>106</v>
@@ -12632,7 +12643,7 @@
         <v>6</v>
       </c>
       <c r="C88" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J88" t="s">
         <v>107</v>
@@ -12650,7 +12661,7 @@
         <v>6</v>
       </c>
       <c r="C89" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J89" t="s">
         <v>108</v>
@@ -12668,7 +12679,7 @@
         <v>191</v>
       </c>
       <c r="C90" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J90" t="s">
         <v>110</v>
@@ -12686,7 +12697,7 @@
         <v>137</v>
       </c>
       <c r="C91" s="26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J91" t="s">
         <v>111</v>
@@ -12704,7 +12715,7 @@
         <v>68</v>
       </c>
       <c r="C92" s="26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J92" t="s">
         <v>112</v>
@@ -12722,10 +12733,10 @@
         <v>15</v>
       </c>
       <c r="C93" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J93" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K93">
         <v>1</v>
@@ -12733,7 +12744,7 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B94" s="1">
         <f t="shared" ref="B94:B101" si="2">VLOOKUP(A94,J:K,2,0)</f>
@@ -12748,7 +12759,7 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B95" s="1">
         <f t="shared" si="2"/>
@@ -12763,7 +12774,7 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B96" s="1">
         <f t="shared" si="2"/>
@@ -12772,7 +12783,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B97" s="1">
         <f t="shared" si="2"/>
@@ -12781,7 +12792,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B98" s="1">
         <f t="shared" si="2"/>
@@ -12790,7 +12801,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B99" s="1">
         <f t="shared" si="2"/>
@@ -12799,7 +12810,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B100" s="1">
         <f t="shared" si="2"/>
@@ -12808,7 +12819,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B101" s="1">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
Se agrega Lago Alberto
</commit_message>
<xml_diff>
--- a/src/Reporte_Discovery.xlsx
+++ b/src/Reporte_Discovery.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jesusarellano/Documents/AXONIUS/Desarrollo/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECE6EBE-F012-4C4F-9FE0-1EFEC8D401DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F54473B-FD07-504B-AEF9-CB4A72EE54F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="9" xr2:uid="{F6E7C25F-76F7-4D4B-8233-292C3B48EDEA}"/>
+    <workbookView xWindow="-10840" yWindow="-22040" windowWidth="30240" windowHeight="18880" xr2:uid="{F6E7C25F-76F7-4D4B-8233-292C3B48EDEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
@@ -53,9 +53,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="149">
   <si>
-    <t>Total Dispositivos descubiertos</t>
-  </si>
-  <si>
     <t>Total Servidores</t>
   </si>
   <si>
@@ -561,6 +558,9 @@
   </si>
   <si>
     <t> Digital View se enfoca en la visualización de datos de redes, servidores, almacenamiento y otros componentes de infraestructura, proporcionando herramientas para la supervisión, diagnóstico y análisis proactivo de posibles problemas.</t>
+  </si>
+  <si>
+    <t>Total Dispositivos y/o Direcciones IPs Descubiertos</t>
   </si>
 </sst>
 </file>
@@ -945,6 +945,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1041,67 +1075,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1516,8 +1516,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:E21"/>
   <sheetViews>
-    <sheetView zoomScale="216" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="216" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1527,89 +1527,86 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="24">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="35"/>
+      <c r="A3" s="49" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="51"/>
       <c r="E3" s="17">
         <v>7507</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="47"/>
-      <c r="B4" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="38"/>
+      <c r="A4" s="63"/>
+      <c r="B4" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="53"/>
+      <c r="D4" s="54"/>
       <c r="E4" s="19">
         <f>E5+E9+E12+E13</f>
         <v>3729</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="48"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="40"/>
+      <c r="A5" s="64"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="56"/>
       <c r="E5" s="20">
         <f>COUNTA(Inventario!B6:B1048576)</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="48"/>
-      <c r="B6" s="51"/>
-      <c r="C6" s="41"/>
+      <c r="A6" s="64"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="64"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="22" t="e">
-        <f>COUNTIF(Inventario!#REF!,"SINO")+COUNTIF(Inventario!#REF!,"SISI")</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="48"/>
-      <c r="B7" s="51"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="22" t="e">
-        <f>COUNTIF(Inventario!#REF!,"NOSI")</f>
-        <v>#REF!</v>
+      <c r="E7" s="22">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="48"/>
-      <c r="B8" s="51"/>
-      <c r="C8" s="43"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="59"/>
       <c r="D8" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="22" t="e">
-        <f>COUNTIF(Inventario!#REF!,"NONO")</f>
-        <v>#REF!</v>
+        <v>22</v>
+      </c>
+      <c r="E8" s="22">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="48"/>
-      <c r="B9" s="51"/>
+      <c r="A9" s="64"/>
+      <c r="B9" s="67"/>
       <c r="C9" s="11"/>
       <c r="D9" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="20">
         <f>COUNTA('Inventario - PC'!B6:B1048576)</f>
@@ -1617,11 +1614,11 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="48"/>
-      <c r="B10" s="51"/>
-      <c r="C10" s="45"/>
+      <c r="A10" s="64"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="61"/>
       <c r="D10" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" s="22">
         <f>COUNTIF('Inventario - PC'!F6:F1048576,"SI")</f>
@@ -1629,11 +1626,11 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="48"/>
-      <c r="B11" s="51"/>
-      <c r="C11" s="46"/>
+      <c r="A11" s="64"/>
+      <c r="B11" s="67"/>
+      <c r="C11" s="62"/>
       <c r="D11" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E11" s="22">
         <f>COUNTIF('Inventario - PC'!F6:F1048576,"no")</f>
@@ -1641,22 +1638,22 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="48"/>
-      <c r="B12" s="51"/>
+      <c r="A12" s="64"/>
+      <c r="B12" s="67"/>
       <c r="C12" s="13"/>
       <c r="D12" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12" s="20">
         <v>3726</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="48"/>
-      <c r="B13" s="52"/>
+      <c r="A13" s="64"/>
+      <c r="B13" s="68"/>
       <c r="C13" s="13"/>
       <c r="D13" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E13" s="20">
         <f>COUNTA('Inventario Identificados'!A5:A1048576)</f>
@@ -1664,24 +1661,24 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="48"/>
-      <c r="B14" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
+      <c r="A14" s="64"/>
+      <c r="B14" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
       <c r="E14" s="21">
         <f>COUNTA('Inventario No Identificados'!A5:A1048576)</f>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="49"/>
-      <c r="B15" s="44" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
+      <c r="A15" s="65"/>
+      <c r="B15" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
       <c r="E15" s="21">
         <f>E3-E4-E14</f>
         <v>3777</v>
@@ -1694,39 +1691,39 @@
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" ht="24">
-      <c r="A18" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
+      <c r="A18" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="46"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="29" t="s">
+      <c r="B20" s="46"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="31"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="47"/>
       <c r="E21" s="5"/>
     </row>
   </sheetData>
@@ -1749,12 +1746,15 @@
   <hyperlinks>
     <hyperlink ref="E9" location="'Inventario - PC'!A1" display="'Inventario - PC'!A1" xr:uid="{0DFC20D2-EC8C-E747-B690-87E905C24920}"/>
     <hyperlink ref="E5" location="Inventario!A1" display="Inventario!A1" xr:uid="{AC498F9B-A70A-FC46-8C40-0AF85EBD504E}"/>
-    <hyperlink ref="E10" location="'Inventario - PC CARSO'!A1" display="'Inventario - PC CARSO'!A1" xr:uid="{C3DB093C-FD53-8345-893E-54AE37D247D8}"/>
-    <hyperlink ref="E11" location="'Inventario - PC CARSO'!A1" display="'Inventario - PC CARSO'!A1" xr:uid="{3F18461C-E759-7D45-A6FA-468FBD08CA6A}"/>
+    <hyperlink ref="E10" location="'Inventario - PC'!A1" display="'Inventario - PC'!A1" xr:uid="{C3DB093C-FD53-8345-893E-54AE37D247D8}"/>
+    <hyperlink ref="E11" location="'Inventario - PC'!A1" display="'Inventario - PC'!A1" xr:uid="{3F18461C-E759-7D45-A6FA-468FBD08CA6A}"/>
     <hyperlink ref="E6:E8" location="'Inventario - CARSO'!A1" display="'Inventario - CARSO'!A1" xr:uid="{DBCEC83B-70F1-E743-8639-7801983E782E}"/>
     <hyperlink ref="E12" location="'Inventario - Red'!A1" display="'Inventario - Red'!A1" xr:uid="{CBA6A172-1EA2-E44C-99A0-76417203F0C8}"/>
     <hyperlink ref="E13" location="'Identificados (OTROS)'!A1" display="'Identificados (OTROS)'!A1" xr:uid="{08D5CB02-FE5D-BC40-954C-F661349E01AC}"/>
     <hyperlink ref="E14" location="'No Identificados'!A1" display="'No Identificados'!A1" xr:uid="{51929993-77DF-9B4E-9D5F-0950FEF690A6}"/>
+    <hyperlink ref="E6" location="Inventario!A1" display="Inventario!A1" xr:uid="{AEB6CA99-9199-084E-8306-67BEE1E4186E}"/>
+    <hyperlink ref="E7" location="Inventario!A1" display="Inventario!A1" xr:uid="{A9DD6EF5-B918-0041-8348-66AEECFBF562}"/>
+    <hyperlink ref="E8" location="Inventario!A1" display="Inventario!A1" xr:uid="{6CCD29C2-D04A-5341-8B0F-B60B531CF83C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1764,566 +1764,566 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F768C478-D652-1F40-804C-166DDCC97E6F}">
   <dimension ref="B2:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="67" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F30" sqref="F30:F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="49.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="65" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5" style="65" customWidth="1"/>
-    <col min="5" max="5" width="27.6640625" style="65" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="112.5" style="65" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="242" style="65" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="33" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5" style="33" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="112.5" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="242" style="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="19">
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="D2" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="61" t="s">
+      <c r="E2" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="61" t="s">
+      <c r="F2" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="61" t="s">
+      <c r="G2" s="29" t="s">
         <v>55</v>
-      </c>
-      <c r="G2" s="61" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="62" t="s">
+      <c r="D3" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="62" t="s">
+      <c r="E3" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="63" t="s">
+      <c r="F3" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="64" t="s">
+      <c r="G3" s="31" t="s">
         <v>61</v>
-      </c>
-      <c r="G3" s="63" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="62"/>
-      <c r="D4" s="65" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="30"/>
+      <c r="D4" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="63" t="s">
+      <c r="F4" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" s="63" t="s">
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="77" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="2:7">
-      <c r="B5" s="66" t="s">
+      <c r="C5" s="30"/>
+      <c r="D5" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="67" t="s">
+      <c r="E5" s="80" t="s">
         <v>67</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="F5" s="83" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="80" t="s">
         <v>68</v>
       </c>
-      <c r="F5" s="69" t="s">
-        <v>61</v>
-      </c>
-      <c r="G5" s="68" t="s">
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="78"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="35" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="6" spans="2:7">
-      <c r="B6" s="70"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="71" t="s">
+      <c r="E6" s="81"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="81"/>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="78"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="72"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="72"/>
-    </row>
-    <row r="7" spans="2:7">
-      <c r="B7" s="70"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="67" t="s">
+      <c r="E7" s="81"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="81"/>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="79"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="72"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="72"/>
-    </row>
-    <row r="8" spans="2:7">
-      <c r="B8" s="74"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="75" t="s">
+      <c r="E8" s="82"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="82"/>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="30"/>
+      <c r="D9" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="E8" s="76"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="76"/>
-    </row>
-    <row r="9" spans="2:7">
-      <c r="B9" s="78" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="62"/>
-      <c r="D9" s="67" t="s">
+      <c r="E9" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="E9" s="79" t="s">
+      <c r="F9" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="38" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="77" t="s">
         <v>74</v>
       </c>
-      <c r="F9" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" s="80" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7">
-      <c r="B10" s="66" t="s">
+      <c r="C10" s="30"/>
+      <c r="D10" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="62"/>
-      <c r="D10" s="67" t="s">
+      <c r="E10" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="68" t="s">
+      <c r="F10" s="83" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="80" t="s">
         <v>77</v>
       </c>
-      <c r="F10" s="69" t="s">
-        <v>61</v>
-      </c>
-      <c r="G10" s="68" t="s">
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="79"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="34" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="11" spans="2:7">
-      <c r="B11" s="74"/>
-      <c r="C11" s="62"/>
-      <c r="D11" s="67" t="s">
+      <c r="E11" s="82"/>
+      <c r="F11" s="85"/>
+      <c r="G11" s="82"/>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="76"/>
-      <c r="F11" s="77"/>
-      <c r="G11" s="76"/>
-    </row>
-    <row r="12" spans="2:7">
-      <c r="B12" s="81" t="s">
+      <c r="C12" s="30"/>
+      <c r="D12" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="62"/>
-      <c r="D12" s="67" t="s">
+      <c r="E12" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="E12" s="82" t="s">
+      <c r="F12" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="F12" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" s="82" t="s">
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="40" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="13" spans="2:7">
-      <c r="B13" s="81" t="s">
+      <c r="C13" s="30"/>
+      <c r="D13" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="62"/>
-      <c r="D13" s="67" t="s">
+      <c r="E13" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="82" t="s">
-        <v>82</v>
-      </c>
-      <c r="F13" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="G13" s="82" t="s">
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14" s="40" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="14" spans="2:7">
-      <c r="B14" s="81" t="s">
+      <c r="C14" s="30"/>
+      <c r="D14" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="62"/>
-      <c r="D14" s="83" t="s">
+      <c r="E14" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="E14" s="82" t="s">
+      <c r="F14" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="41" t="s">
         <v>89</v>
-      </c>
-      <c r="F14" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="G14" s="82" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="15" spans="2:7">
       <c r="B15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="30"/>
+      <c r="D15" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="C15" s="62"/>
-      <c r="D15" s="67" t="s">
+      <c r="E15" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="E15" s="80" t="s">
+      <c r="F15" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="38" t="s">
         <v>93</v>
-      </c>
-      <c r="F15" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="80" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="16" spans="2:7">
       <c r="B16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="62"/>
-      <c r="D16" s="67" t="s">
+      <c r="E16" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="41" t="s">
         <v>96</v>
-      </c>
-      <c r="E16" s="82" t="s">
-        <v>89</v>
-      </c>
-      <c r="F16" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="G16" s="82" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="17" spans="2:7">
       <c r="B17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="62"/>
-      <c r="D17" s="67" t="s">
+      <c r="E17" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="43" t="s">
         <v>99</v>
-      </c>
-      <c r="E17" s="84" t="s">
-        <v>89</v>
-      </c>
-      <c r="F17" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="G17" s="84" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="18" spans="2:7">
       <c r="B18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="30"/>
+      <c r="D18" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="67" t="s">
+      <c r="E18" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="E18" s="84" t="s">
-        <v>89</v>
-      </c>
-      <c r="F18" s="62" t="s">
+      <c r="G18" s="43" t="s">
         <v>103</v>
-      </c>
-      <c r="G18" s="84" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="19" spans="2:7">
       <c r="B19" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62" t="s">
+      <c r="E19" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="E19" s="84" t="s">
+      <c r="F19" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" s="43" t="s">
         <v>107</v>
-      </c>
-      <c r="F19" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="G19" s="84" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="20" spans="2:7">
       <c r="B20" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="C20" s="62"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="84" t="s">
+      <c r="F20" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="F20" s="85" t="s">
+      <c r="G20" s="43" t="s">
         <v>111</v>
-      </c>
-      <c r="G20" s="84" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="18">
       <c r="B21" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="F21" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="G21" s="43" t="s">
         <v>113</v>
-      </c>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="84" t="s">
-        <v>110</v>
-      </c>
-      <c r="F21" s="85" t="s">
-        <v>111</v>
-      </c>
-      <c r="G21" s="84" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="22" spans="2:7">
       <c r="B22" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="G22" s="43" t="s">
         <v>115</v>
-      </c>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="84" t="s">
-        <v>110</v>
-      </c>
-      <c r="F22" s="85" t="s">
-        <v>111</v>
-      </c>
-      <c r="G22" s="84" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="18">
       <c r="B23" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62" t="s">
+      <c r="F23" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="G23" s="30" t="s">
         <v>118</v>
-      </c>
-      <c r="F23" s="85" t="s">
-        <v>111</v>
-      </c>
-      <c r="G23" s="62" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="24" spans="2:7">
       <c r="B24" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C24" s="62"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="62" t="s">
-        <v>118</v>
-      </c>
-      <c r="F24" s="85" t="s">
-        <v>111</v>
-      </c>
-      <c r="G24" s="62"/>
+        <v>119</v>
+      </c>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="F24" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="G24" s="30"/>
     </row>
     <row r="25" spans="2:7">
       <c r="B25" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="F25" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="G25" s="30" t="s">
         <v>121</v>
-      </c>
-      <c r="C25" s="62"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="62" t="s">
-        <v>118</v>
-      </c>
-      <c r="F25" s="85" t="s">
-        <v>111</v>
-      </c>
-      <c r="G25" s="62" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="26" spans="2:7">
       <c r="B26" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="F26" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62" t="s">
-        <v>118</v>
-      </c>
-      <c r="F26" s="62" t="s">
+      <c r="G26" s="30" t="s">
         <v>124</v>
-      </c>
-      <c r="G26" s="62" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="16" customHeight="1">
       <c r="B27" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="F27" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="G27" s="30" t="s">
         <v>126</v>
-      </c>
-      <c r="C27" s="62"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="62" t="s">
-        <v>118</v>
-      </c>
-      <c r="F27" s="85" t="s">
-        <v>111</v>
-      </c>
-      <c r="G27" s="62" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="28" spans="2:7">
       <c r="B28" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="C28" s="62"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="62" t="s">
+      <c r="F28" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="F28" s="62" t="s">
+      <c r="G28" s="30" t="s">
         <v>130</v>
-      </c>
-      <c r="G28" s="62" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="29" spans="2:7">
       <c r="B29" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="C29" s="62"/>
-      <c r="D29" s="62" t="s">
+      <c r="E29" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="E29" s="62" t="s">
+      <c r="F29" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="G29" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="F29" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="G29" s="62" t="s">
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" s="77" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="30" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="30" spans="2:7">
-      <c r="B30" s="66" t="s">
-        <v>66</v>
-      </c>
-      <c r="C30" s="62" t="s">
+      <c r="D30" s="40" t="s">
         <v>136</v>
       </c>
-      <c r="D30" s="81" t="s">
+      <c r="E30" s="80" t="s">
         <v>137</v>
       </c>
-      <c r="E30" s="68" t="s">
+      <c r="F30" s="83" t="s">
+        <v>60</v>
+      </c>
+      <c r="G30" s="80" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7">
+      <c r="B31" s="78"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="F30" s="69" t="s">
-        <v>61</v>
-      </c>
-      <c r="G30" s="68" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7">
-      <c r="B31" s="70"/>
-      <c r="C31" s="62"/>
-      <c r="D31" s="81" t="s">
+      <c r="E31" s="81"/>
+      <c r="F31" s="84"/>
+      <c r="G31" s="81"/>
+    </row>
+    <row r="32" spans="2:7">
+      <c r="B32" s="79"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="40" t="s">
         <v>139</v>
       </c>
-      <c r="E31" s="72"/>
-      <c r="F31" s="73"/>
-      <c r="G31" s="72"/>
-    </row>
-    <row r="32" spans="2:7">
-      <c r="B32" s="74"/>
-      <c r="C32" s="62"/>
-      <c r="D32" s="81" t="s">
-        <v>140</v>
-      </c>
-      <c r="E32" s="76"/>
-      <c r="F32" s="77"/>
-      <c r="G32" s="76"/>
+      <c r="E32" s="82"/>
+      <c r="F32" s="85"/>
+      <c r="G32" s="82"/>
     </row>
     <row r="33" spans="2:7">
       <c r="B33" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="C33" s="62"/>
-      <c r="D33" s="62" t="s">
+      <c r="E33" s="41" t="s">
         <v>142</v>
       </c>
-      <c r="E33" s="82" t="s">
+      <c r="F33" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="G33" s="41" t="s">
         <v>143</v>
-      </c>
-      <c r="F33" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="G33" s="82" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="34" spans="2:7">
       <c r="B34" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C34" s="62"/>
-      <c r="D34" s="62" t="s">
+        <v>140</v>
+      </c>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="E34" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="E34" s="82" t="s">
-        <v>146</v>
-      </c>
-      <c r="F34" s="64" t="s">
-        <v>61</v>
-      </c>
-      <c r="G34" s="82" t="s">
-        <v>144</v>
+      <c r="F34" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="G34" s="41" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="2:7">
       <c r="B35" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="C35" s="62"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="82" t="s">
+      <c r="F35" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="F35" s="62" t="s">
+      <c r="G35" s="41" t="s">
         <v>147</v>
-      </c>
-      <c r="G35" s="82" t="s">
-        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2374,66 +2374,66 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:7" ht="24">
-      <c r="A3" s="53" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
+      <c r="A3" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
     </row>
     <row r="4" spans="1:7" ht="16" customHeight="1">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="C4" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="D4" s="70" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="54" t="s">
+      <c r="F4" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="54" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="54" t="s">
-        <v>38</v>
+      <c r="G4" s="70" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="55"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
+      <c r="A5" s="71"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
     </row>
     <row r="6" spans="1:7" ht="17">
       <c r="A6" s="1">
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>31</v>
-      </c>
       <c r="F6" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6" s="8"/>
     </row>
@@ -11504,33 +11504,33 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:6" ht="24" customHeight="1">
-      <c r="A3" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
+      <c r="A3" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
     </row>
     <row r="4" spans="1:6" ht="17">
       <c r="A4" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="C4" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="D4" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>12</v>
-      </c>
       <c r="F4" s="27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17">
@@ -11538,19 +11538,19 @@
         <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>31</v>
-      </c>
       <c r="F5" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -11594,86 +11594,86 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:10" ht="24">
-      <c r="A3" s="53" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
+      <c r="A3" s="69" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="72" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="C4" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="D4" s="70" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="56" t="s">
+      <c r="F4" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="56" t="s">
+      <c r="G4" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="56" t="s">
+      <c r="H4" s="73" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="73"/>
+      <c r="J4" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="57" t="s">
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="72"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="57"/>
-      <c r="J4" s="56" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="56"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" s="56"/>
+      <c r="J5" s="72"/>
     </row>
     <row r="6" spans="1:10" ht="17">
       <c r="A6" s="1">
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="D6" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>19</v>
       </c>
       <c r="H6" s="8">
         <v>0</v>
@@ -11682,7 +11682,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -11731,69 +11731,69 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:11" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A3" s="58" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
+      <c r="A3" s="74" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="75" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="C4" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="56" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="59" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="59" t="s">
-        <v>40</v>
+      <c r="D4" s="70" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="70" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="75" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="70" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="75" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="59"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="59"/>
+      <c r="A5" s="75"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="75"/>
     </row>
     <row r="6" spans="1:11" ht="34">
       <c r="A6" s="23">
         <v>1</v>
       </c>
       <c r="B6" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="26" t="s">
         <v>41</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>42</v>
       </c>
       <c r="D6" s="26"/>
       <c r="E6" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="23"/>
@@ -11836,29 +11836,29 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="24">
-      <c r="A3" s="53" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
+      <c r="A3" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
     </row>
     <row r="4" spans="1:5" ht="17">
       <c r="A4" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="C4" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="D4" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="27" t="s">
         <v>11</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17">
@@ -11866,16 +11866,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -11913,29 +11913,29 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="24">
-      <c r="A3" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
+      <c r="A3" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
     </row>
     <row r="4" spans="1:5" ht="17">
       <c r="A4" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="C4" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="D4" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="27" t="s">
         <v>11</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17">
@@ -11943,16 +11943,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug Fixed EoL Inventario - EOL
</commit_message>
<xml_diff>
--- a/src/Reporte_Discovery.xlsx
+++ b/src/Reporte_Discovery.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10817"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jesusarellano/Documents/TELCEL/AXONIUS/Desarrollo/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C8A8B5-9808-8044-A2AE-464ABC165276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D297A38-B948-B04F-B2DF-E69D4F6FBE3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16180" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="143">
   <si>
     <t>Adaptador</t>
   </si>
@@ -475,16 +475,6 @@
   </si>
   <si>
     <t>Software EoL</t>
-  </si>
-  <si>
-    <t>ITHHWHUEPRO17</t>
-  </si>
-  <si>
-    <t>10.119.249.106
-138.1.1.126</t>
-  </si>
-  <si>
-    <t>Linux Red Hat 7.9</t>
   </si>
   <si>
     <t xml:space="preserve">Servidores CARSO - Inventario </t>
@@ -1132,6 +1122,24 @@
     <xf numFmtId="3" fontId="13" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1140,6 +1148,135 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1167,153 +1304,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1629,8 +1619,8 @@
   </sheetPr>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="298" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="A9" zoomScale="218" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1650,82 +1640,82 @@
       <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" s="18" customFormat="1" ht="24">
-      <c r="A2" s="61"/>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="62"/>
+      <c r="A2" s="64"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="65"/>
     </row>
     <row r="3" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A3" s="63" t="s">
-        <v>126</v>
-      </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="65"/>
+      <c r="A3" s="85" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="86"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="87"/>
       <c r="F3" s="41">
         <v>7507</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A4" s="72"/>
-      <c r="B4" s="66" t="s">
-        <v>127</v>
-      </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="68"/>
+      <c r="A4" s="66"/>
+      <c r="B4" s="74" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="76"/>
       <c r="F4" s="42">
         <f>F5+F10+F13+F14</f>
         <v>3728</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A5" s="73"/>
-      <c r="B5" s="74"/>
-      <c r="C5" s="69" t="s">
-        <v>128</v>
-      </c>
-      <c r="D5" s="70"/>
-      <c r="E5" s="71"/>
+      <c r="A5" s="67"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="80" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" s="81"/>
+      <c r="E5" s="82"/>
       <c r="F5" s="44">
         <f>COUNTA(Inventario!B6:B1048576)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A6" s="73"/>
-      <c r="B6" s="75"/>
-      <c r="C6" s="76"/>
-      <c r="D6" s="77" t="s">
-        <v>129</v>
-      </c>
-      <c r="E6" s="78"/>
+      <c r="A6" s="67"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="53" t="s">
+        <v>126</v>
+      </c>
+      <c r="E6" s="54"/>
       <c r="F6" s="45">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A7" s="73"/>
-      <c r="B7" s="75"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="77" t="s">
-        <v>141</v>
-      </c>
-      <c r="E7" s="78"/>
+      <c r="A7" s="67"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="53" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7" s="54"/>
       <c r="F7" s="45">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A8" s="73"/>
-      <c r="B8" s="75"/>
-      <c r="C8" s="79"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="80" t="s">
-        <v>142</v>
+      <c r="A8" s="67"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="49" t="s">
+        <v>139</v>
       </c>
       <c r="F8" s="46">
         <f>F7-F9</f>
@@ -1733,12 +1723,12 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A9" s="73"/>
-      <c r="B9" s="75"/>
-      <c r="C9" s="81"/>
-      <c r="D9" s="82"/>
-      <c r="E9" s="80" t="s">
-        <v>143</v>
+      <c r="A9" s="67"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="49" t="s">
+        <v>140</v>
       </c>
       <c r="F9" s="47" cm="1">
         <f t="array" ref="F9">SUM(COUNTIFS(Inventario!E6:E1048576, {"Oracle Solaris","Windows Server 2008 R2","Windows Server 2003 R2","SunOS 10","SunOS 11.1","SunOS 11.2","SunOS 11.3","IBM AIX 6.1","IBM AIX 7.1","IBM AIX 7.2","IBM AIX 5.3","SunOS 9","SunOS 11.4.23.69.3","SunOS 11.0","SunOS 11.4","SunOS 11.4.0.15.0"}, Inventario!F6:F1048576, "NO"))</f>
@@ -1746,90 +1736,90 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A10" s="73"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="69" t="s">
-        <v>130</v>
-      </c>
-      <c r="D10" s="70"/>
-      <c r="E10" s="71"/>
+      <c r="A10" s="67"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="80" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="81"/>
+      <c r="E10" s="82"/>
       <c r="F10" s="44">
         <f>COUNTA('Inventario - PC'!B6:B1048576)</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A11" s="73"/>
-      <c r="B11" s="75"/>
-      <c r="C11" s="83"/>
-      <c r="D11" s="84" t="s">
-        <v>131</v>
-      </c>
-      <c r="E11" s="85"/>
+      <c r="A11" s="67"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="83" t="s">
+        <v>128</v>
+      </c>
+      <c r="E11" s="84"/>
       <c r="F11" s="46">
         <f>COUNTIF('Inventario - PC'!F6:F1048576,"SI")</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A12" s="73"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="84" t="s">
-        <v>132</v>
-      </c>
-      <c r="E12" s="85"/>
+      <c r="A12" s="67"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="83" t="s">
+        <v>129</v>
+      </c>
+      <c r="E12" s="84"/>
       <c r="F12" s="46">
         <f>COUNTIF('Inventario - PC'!F6:F1048576,"no")</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A13" s="73"/>
-      <c r="B13" s="75"/>
-      <c r="C13" s="69" t="s">
-        <v>133</v>
-      </c>
-      <c r="D13" s="70"/>
-      <c r="E13" s="71"/>
+      <c r="A13" s="67"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="80" t="s">
+        <v>130</v>
+      </c>
+      <c r="D13" s="81"/>
+      <c r="E13" s="82"/>
       <c r="F13" s="44">
         <v>3726</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A14" s="73"/>
-      <c r="B14" s="82"/>
-      <c r="C14" s="69" t="s">
-        <v>134</v>
-      </c>
-      <c r="D14" s="70"/>
-      <c r="E14" s="71"/>
+      <c r="A14" s="67"/>
+      <c r="B14" s="71"/>
+      <c r="C14" s="80" t="s">
+        <v>131</v>
+      </c>
+      <c r="D14" s="81"/>
+      <c r="E14" s="82"/>
       <c r="F14" s="44">
         <f>COUNTA('Inventario Identificados'!A5:A1048576)</f>
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A15" s="73"/>
-      <c r="B15" s="66" t="s">
-        <v>135</v>
-      </c>
-      <c r="C15" s="67"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="68"/>
+      <c r="A15" s="67"/>
+      <c r="B15" s="74" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" s="75"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="76"/>
       <c r="F15" s="48">
         <f>COUNTA('Inventario No Identificados'!A5:A1048576)</f>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A16" s="87"/>
-      <c r="B16" s="66" t="s">
-        <v>136</v>
-      </c>
-      <c r="C16" s="67"/>
-      <c r="D16" s="67"/>
-      <c r="E16" s="68"/>
+      <c r="A16" s="68"/>
+      <c r="B16" s="74" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" s="75"/>
+      <c r="D16" s="75"/>
+      <c r="E16" s="76"/>
       <c r="F16" s="42">
         <f>F3-F4-F15</f>
         <v>3778</v>
@@ -1852,62 +1842,53 @@
       <c r="F18" s="43"/>
     </row>
     <row r="19" spans="1:6" s="18" customFormat="1" ht="24">
-      <c r="A19" s="88" t="s">
+      <c r="A19" s="58" t="s">
+        <v>134</v>
+      </c>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="60"/>
+    </row>
+    <row r="20" spans="1:6" ht="17.25" customHeight="1">
+      <c r="A20" s="61" t="s">
+        <v>135</v>
+      </c>
+      <c r="B20" s="62"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="55" t="s">
+        <v>141</v>
+      </c>
+      <c r="F20" s="56"/>
+    </row>
+    <row r="21" spans="1:6" ht="17.25" customHeight="1">
+      <c r="A21" s="61" t="s">
+        <v>136</v>
+      </c>
+      <c r="B21" s="62"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="55" t="s">
+        <v>141</v>
+      </c>
+      <c r="F21" s="56"/>
+    </row>
+    <row r="22" spans="1:6" ht="17.25" customHeight="1">
+      <c r="A22" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="B19" s="89"/>
-      <c r="C19" s="89"/>
-      <c r="D19" s="89"/>
-      <c r="E19" s="89"/>
-      <c r="F19" s="90"/>
-    </row>
-    <row r="20" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A20" s="91" t="s">
-        <v>138</v>
-      </c>
-      <c r="B20" s="92"/>
-      <c r="C20" s="92"/>
-      <c r="D20" s="93"/>
-      <c r="E20" s="49" t="s">
-        <v>144</v>
-      </c>
-      <c r="F20" s="50"/>
-    </row>
-    <row r="21" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A21" s="91" t="s">
-        <v>139</v>
-      </c>
-      <c r="B21" s="92"/>
-      <c r="C21" s="92"/>
-      <c r="D21" s="93"/>
-      <c r="E21" s="49" t="s">
-        <v>144</v>
-      </c>
-      <c r="F21" s="50"/>
-    </row>
-    <row r="22" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A22" s="91" t="s">
-        <v>140</v>
-      </c>
-      <c r="B22" s="92"/>
-      <c r="C22" s="92"/>
-      <c r="D22" s="93"/>
-      <c r="E22" s="51" t="s">
-        <v>145</v>
-      </c>
-      <c r="F22" s="50"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="57" t="s">
+        <v>142</v>
+      </c>
+      <c r="F22" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A4:A16"/>
     <mergeCell ref="B5:B14"/>
@@ -1924,6 +1905,15 @@
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="C5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F5" location="Inventario!A1" display="Inventario!A1" xr:uid="{B80F5769-9041-D946-A663-3C05C393B9EF}"/>
@@ -2025,52 +2015,52 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="101" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="104" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="58" t="s">
+      <c r="F5" s="107" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="55" t="s">
+      <c r="G5" s="104" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B6" s="53"/>
+      <c r="B6" s="102"/>
       <c r="C6" s="4"/>
       <c r="D6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="56"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="56"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="108"/>
+      <c r="G6" s="105"/>
     </row>
     <row r="7" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B7" s="53"/>
+      <c r="B7" s="102"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="56"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="56"/>
+      <c r="E7" s="105"/>
+      <c r="F7" s="108"/>
+      <c r="G7" s="105"/>
     </row>
     <row r="8" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B8" s="54"/>
+      <c r="B8" s="103"/>
       <c r="C8" s="4"/>
       <c r="D8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="57"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="57"/>
+      <c r="E8" s="106"/>
+      <c r="F8" s="109"/>
+      <c r="G8" s="106"/>
     </row>
     <row r="9" spans="2:7" ht="17.25" customHeight="1">
       <c r="B9" s="9" t="s">
@@ -2091,32 +2081,32 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="101" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="55" t="s">
+      <c r="E10" s="104" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="58" t="s">
+      <c r="F10" s="107" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="55" t="s">
+      <c r="G10" s="104" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B11" s="54"/>
+      <c r="B11" s="103"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="57"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="57"/>
+      <c r="E11" s="106"/>
+      <c r="F11" s="109"/>
+      <c r="G11" s="106"/>
     </row>
     <row r="12" spans="2:7" ht="17.25" customHeight="1">
       <c r="B12" s="3" t="s">
@@ -2423,7 +2413,7 @@
       </c>
     </row>
     <row r="30" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B30" s="52" t="s">
+      <c r="B30" s="101" t="s">
         <v>16</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -2432,35 +2422,35 @@
       <c r="D30" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E30" s="55" t="s">
+      <c r="E30" s="104" t="s">
         <v>88</v>
       </c>
-      <c r="F30" s="58" t="s">
+      <c r="F30" s="107" t="s">
         <v>10</v>
       </c>
-      <c r="G30" s="55" t="s">
+      <c r="G30" s="104" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B31" s="53"/>
+      <c r="B31" s="102"/>
       <c r="C31" s="4"/>
       <c r="D31" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E31" s="56"/>
-      <c r="F31" s="59"/>
-      <c r="G31" s="56"/>
+      <c r="E31" s="105"/>
+      <c r="F31" s="108"/>
+      <c r="G31" s="105"/>
     </row>
     <row r="32" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B32" s="54"/>
+      <c r="B32" s="103"/>
       <c r="C32" s="4"/>
       <c r="D32" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E32" s="57"/>
-      <c r="F32" s="60"/>
-      <c r="G32" s="57"/>
+      <c r="E32" s="106"/>
+      <c r="F32" s="109"/>
+      <c r="G32" s="106"/>
     </row>
     <row r="33" spans="2:7" ht="17.25" customHeight="1">
       <c r="B33" s="3" t="s">
@@ -2540,8 +2530,8 @@
   </sheetPr>
   <dimension ref="A1:G2262"/>
   <sheetViews>
-    <sheetView zoomScale="211" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView zoomScale="133" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2565,64 +2555,64 @@
       <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:7" s="18" customFormat="1" ht="24">
-      <c r="A3" s="94" t="s">
-        <v>124</v>
-      </c>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
+      <c r="A3" s="88" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
     </row>
     <row r="4" spans="1:7" s="18" customFormat="1" ht="16" customHeight="1">
-      <c r="A4" s="96" t="s">
+      <c r="A4" s="90" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="97" t="s">
+      <c r="B4" s="92" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="97" t="s">
+      <c r="C4" s="92" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="97" t="s">
+      <c r="D4" s="92" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="97" t="s">
+      <c r="E4" s="92" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="97" t="s">
+      <c r="F4" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="97" t="s">
+      <c r="G4" s="92" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="18" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A5" s="98"/>
-      <c r="B5" s="99"/>
-      <c r="C5" s="99"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
+      <c r="A5" s="91"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="93"/>
     </row>
     <row r="6" spans="1:7" ht="17.25" customHeight="1">
       <c r="A6" s="19"/>
       <c r="B6" s="37" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E6" s="39" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F6" s="39" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G6" s="21"/>
     </row>
@@ -13959,32 +13949,32 @@
       <c r="F2" s="17"/>
     </row>
     <row r="3" spans="1:6" s="18" customFormat="1" ht="24">
-      <c r="A3" s="94" t="s">
-        <v>123</v>
-      </c>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
+      <c r="A3" s="88" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
     </row>
     <row r="4" spans="1:6" s="18" customFormat="1" ht="17">
-      <c r="A4" s="100" t="s">
+      <c r="A4" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="101" t="s">
+      <c r="C4" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="101" t="s">
+      <c r="D4" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="101" t="s">
+      <c r="E4" s="51" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="101" t="s">
+      <c r="F4" s="51" t="s">
         <v>104</v>
       </c>
     </row>
@@ -14065,64 +14055,64 @@
       <c r="J2" s="17"/>
     </row>
     <row r="3" spans="1:10" s="18" customFormat="1" ht="24">
-      <c r="A3" s="94" t="s">
+      <c r="A3" s="88" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="89"/>
+    </row>
+    <row r="4" spans="1:10" s="18" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A4" s="90" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="92" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="92" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="92" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="92" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="92" t="s">
+        <v>115</v>
+      </c>
+      <c r="H4" s="94" t="s">
+        <v>116</v>
+      </c>
+      <c r="I4" s="94"/>
+      <c r="J4" s="92" t="s">
         <v>117</v>
       </c>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="94"/>
-      <c r="J3" s="95"/>
-    </row>
-    <row r="4" spans="1:10" s="18" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A4" s="96" t="s">
-        <v>100</v>
-      </c>
-      <c r="B4" s="97" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="97" t="s">
-        <v>102</v>
-      </c>
-      <c r="D4" s="97" t="s">
-        <v>103</v>
-      </c>
-      <c r="E4" s="97" t="s">
-        <v>104</v>
-      </c>
-      <c r="F4" s="97" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="97" t="s">
+    </row>
+    <row r="5" spans="1:10" ht="17.25" customHeight="1">
+      <c r="A5" s="91"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="93"/>
+      <c r="H5" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="H4" s="102" t="s">
+      <c r="I5" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="I4" s="102"/>
-      <c r="J4" s="97" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A5" s="98"/>
-      <c r="B5" s="99"/>
-      <c r="C5" s="99"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="103" t="s">
-        <v>121</v>
-      </c>
-      <c r="I5" s="103" t="s">
-        <v>122</v>
-      </c>
-      <c r="J5" s="99"/>
+      <c r="J5" s="93"/>
     </row>
     <row r="6" spans="1:10" ht="18.75" customHeight="1">
       <c r="A6" s="19"/>
@@ -14161,8 +14151,8 @@
   </sheetPr>
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -14196,75 +14186,65 @@
       <c r="H2" s="25"/>
     </row>
     <row r="3" spans="1:11" s="18" customFormat="1" ht="24">
-      <c r="A3" s="104" t="s">
+      <c r="A3" s="95" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="105"/>
-      <c r="C3" s="105"/>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="105"/>
-      <c r="H3" s="104"/>
+      <c r="B3" s="96"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="95"/>
       <c r="I3" s="27"/>
       <c r="J3" s="27"/>
       <c r="K3" s="27"/>
     </row>
     <row r="4" spans="1:11" ht="17.25" customHeight="1">
-      <c r="A4" s="106" t="s">
+      <c r="A4" s="97" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="98" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="108" t="s">
+      <c r="C4" s="99" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="97" t="s">
+      <c r="D4" s="92" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="97" t="s">
+      <c r="E4" s="92" t="s">
         <v>111</v>
       </c>
-      <c r="F4" s="109" t="s">
+      <c r="F4" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="97" t="s">
+      <c r="G4" s="92" t="s">
         <v>112</v>
       </c>
-      <c r="H4" s="106" t="s">
+      <c r="H4" s="97" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="17.25" customHeight="1">
-      <c r="A5" s="106"/>
-      <c r="B5" s="107"/>
-      <c r="C5" s="108"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="109"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="106"/>
+      <c r="A5" s="97"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="99"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="93"/>
+      <c r="H5" s="97"/>
     </row>
     <row r="6" spans="1:11" ht="17.25" customHeight="1">
-      <c r="A6" s="28">
-        <v>1</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>115</v>
-      </c>
+      <c r="A6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="30"/>
-      <c r="E6" s="30" t="s">
-        <v>116</v>
-      </c>
+      <c r="E6" s="30"/>
       <c r="F6" s="29"/>
       <c r="G6" s="29"/>
-      <c r="H6" s="28">
-        <v>10</v>
-      </c>
+      <c r="H6" s="28"/>
     </row>
   </sheetData>
   <autoFilter ref="A4:H5" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
@@ -14318,28 +14298,28 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:5" s="18" customFormat="1" ht="24">
-      <c r="A3" s="94" t="s">
+      <c r="A3" s="88" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
     </row>
     <row r="4" spans="1:5" s="18" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A4" s="100" t="s">
+      <c r="A4" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="101" t="s">
+      <c r="C4" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="101" t="s">
+      <c r="D4" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="101" t="s">
+      <c r="E4" s="51" t="s">
         <v>104</v>
       </c>
     </row>
@@ -14404,28 +14384,28 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:5" s="18" customFormat="1" ht="24">
-      <c r="A3" s="94" t="s">
+      <c r="A3" s="88" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
     </row>
     <row r="4" spans="1:5" s="18" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A4" s="100" t="s">
+      <c r="A4" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="101" t="s">
+      <c r="C4" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="101" t="s">
+      <c r="D4" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="101" t="s">
+      <c r="E4" s="51" t="s">
         <v>104</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bug resolved: # Exceeded
</commit_message>
<xml_diff>
--- a/src/Reporte_Discovery.xlsx
+++ b/src/Reporte_Discovery.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11018"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jesusarellano/Documents/TELCEL/AXONIUS/Desarrollo/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA1AD75-A6F3-424B-9AB8-1B4BD374ABC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D62153-727F-3649-9BBE-0CD394AA4CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="17120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,6 +34,10 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Inventario No Identificados'!$A$4:$E$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="91" r:id="rId11"/>
+    <pivotCache cacheId="92" r:id="rId12"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -73,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="153">
   <si>
     <t>Adaptador</t>
   </si>
@@ -563,12 +567,42 @@
   <si>
     <t>Inventario - EOL'!A1</t>
   </si>
+  <si>
+    <t>Adaptadores</t>
+  </si>
+  <si>
+    <t>IPs</t>
+  </si>
+  <si>
+    <t>MACs</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Clasificacion</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Count of Clasificacion</t>
+  </si>
+  <si>
+    <t>(blank)</t>
+  </si>
+  <si>
+    <t>Window</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -678,6 +712,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -995,7 +1035,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1133,11 +1173,57 @@
     <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="13" fillId="9" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="10" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="13" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1172,6 +1258,12 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1181,6 +1273,21 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1189,6 +1296,15 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="6" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1256,72 +1372,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="9" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="10" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="13" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1344,6 +1394,206 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jesús Arellano" refreshedDate="46008.610441550925" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="2" xr:uid="{74DEB354-E178-9942-86C6-D9C6DB3B4B64}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A4:E1048576" sheet="Inventario Identificados"/>
+  </cacheSource>
+  <cacheFields count="5">
+    <cacheField name="Adaptadores" numFmtId="3">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="1"/>
+    </cacheField>
+    <cacheField name="IPs" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="MACs" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Manufacturer" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Clasificacion" numFmtId="0">
+      <sharedItems containsBlank="1" count="2">
+        <s v="Windows 10"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Jesús Arellano" refreshedDate="46008.613557291668" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="2" xr:uid="{833D5FB0-8697-5E4B-8135-AAEDADA852DA}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A4:E1048576" sheet="Inventario No Identificados"/>
+  </cacheSource>
+  <cacheFields count="5">
+    <cacheField name="Adaptadores" numFmtId="3">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="1"/>
+    </cacheField>
+    <cacheField name="IPs" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="MACs" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Manufacturer" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Clasificacion" numFmtId="0">
+      <sharedItems containsBlank="1" count="2">
+        <s v="Windows 10"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="2">
+  <r>
+    <n v="1"/>
+    <s v="SVVUW0106S3MXCO"/>
+    <s v="10.188.60.195"/>
+    <s v="00:90:FB:63:B2:84"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="2">
+  <r>
+    <n v="1"/>
+    <s v="SVVUW0106S3MXCO"/>
+    <s v="10.188.60.195"/>
+    <s v="00:90:FB:63:B2:84"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B0F87A7E-D022-2E4A-8DDE-C4E01F9C3F96}" name="PivotTable1" cacheId="92" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B2:C5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Clasificacion" fld="4" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E7C88826-A921-F241-A7D7-09240D889B29}" name="PivotTable2" cacheId="91" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B2:C5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Clasificacion" fld="4" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1631,7 +1881,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sheet1">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:F22"/>
@@ -1655,189 +1905,189 @@
       <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" s="18" customFormat="1" ht="24">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="48"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="58"/>
     </row>
     <row r="3" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="78" t="s">
         <v>123</v>
       </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="62"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="80"/>
       <c r="F3" s="41">
         <v>7507</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A4" s="88"/>
-      <c r="B4" s="51" t="s">
+      <c r="A4" s="59"/>
+      <c r="B4" s="67" t="s">
         <v>124</v>
       </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="53"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="69"/>
       <c r="F4" s="42">
         <f>F5+F10+F13+F14</f>
-        <v>3728</v>
+        <v>3729</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A5" s="89"/>
-      <c r="B5" s="90"/>
-      <c r="C5" s="57" t="s">
+      <c r="A5" s="60"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="73" t="s">
         <v>125</v>
       </c>
-      <c r="D5" s="58"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="91">
+      <c r="D5" s="74"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="47">
         <f>COUNTA(Inventario!B6:B1048576)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A6" s="89"/>
-      <c r="B6" s="92"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="93" t="s">
+      <c r="A6" s="60"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="81" t="s">
         <v>126</v>
       </c>
-      <c r="E6" s="94"/>
-      <c r="F6" s="95">
+      <c r="E6" s="82"/>
+      <c r="F6" s="48">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A7" s="89"/>
-      <c r="B7" s="92"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="93" t="s">
+      <c r="A7" s="60"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="81" t="s">
         <v>138</v>
       </c>
-      <c r="E7" s="94"/>
-      <c r="F7" s="95">
+      <c r="E7" s="82"/>
+      <c r="F7" s="48">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A8" s="89"/>
-      <c r="B8" s="92"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="90"/>
-      <c r="E8" s="96" t="s">
+      <c r="A8" s="60"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="49" t="s">
         <v>139</v>
       </c>
-      <c r="F8" s="97">
+      <c r="F8" s="50">
         <f>F7-F9</f>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A9" s="89"/>
-      <c r="B9" s="92"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="98"/>
-      <c r="E9" s="96" t="s">
+      <c r="A9" s="60"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="49" t="s">
         <v>140</v>
       </c>
-      <c r="F9" s="99" cm="1">
+      <c r="F9" s="51" cm="1">
         <f t="array" ref="F9">SUM(COUNTIFS(Inventario!E6:E1048576, {"Oracle Solaris","Windows Server 2008 R2","Windows Server 2003 R2","SunOS 10","SunOS 11.1","SunOS 11.2","SunOS 11.3","IBM AIX 6.1","IBM AIX 7.1","IBM AIX 7.2","IBM AIX 5.3","SunOS 9","SunOS 11.4.23.69.3","SunOS 11.0","SunOS 11.4","SunOS 11.4.0.15.0"}, Inventario!F6:F1048576, "NO"))</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A10" s="89"/>
-      <c r="B10" s="92"/>
-      <c r="C10" s="57" t="s">
+      <c r="A10" s="60"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="73" t="s">
         <v>127</v>
       </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="91">
+      <c r="D10" s="74"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="47">
         <f>COUNTA('Inventario - PC'!B6:B1048576)</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A11" s="89"/>
-      <c r="B11" s="92"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="100" t="s">
+      <c r="A11" s="60"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="76" t="s">
         <v>128</v>
       </c>
-      <c r="E11" s="101"/>
-      <c r="F11" s="97">
+      <c r="E11" s="77"/>
+      <c r="F11" s="50">
         <f>COUNTIF('Inventario - PC'!F6:F1048576,"SI")</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A12" s="89"/>
-      <c r="B12" s="92"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="100" t="s">
+      <c r="A12" s="60"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="76" t="s">
         <v>129</v>
       </c>
-      <c r="E12" s="101"/>
-      <c r="F12" s="97">
+      <c r="E12" s="77"/>
+      <c r="F12" s="50">
         <f>COUNTIF('Inventario - PC'!F6:F1048576,"no")</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A13" s="89"/>
-      <c r="B13" s="92"/>
-      <c r="C13" s="57" t="s">
+      <c r="A13" s="60"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="73" t="s">
         <v>130</v>
       </c>
-      <c r="D13" s="58"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="91">
+      <c r="D13" s="74"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="47">
         <v>3726</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A14" s="89"/>
-      <c r="B14" s="98"/>
-      <c r="C14" s="57" t="s">
+      <c r="A14" s="60"/>
+      <c r="B14" s="64"/>
+      <c r="C14" s="73" t="s">
         <v>131</v>
       </c>
-      <c r="D14" s="58"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="91">
+      <c r="D14" s="74"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="47">
         <f>COUNTA('Inventario Identificados'!A5:A1048576)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A15" s="89"/>
-      <c r="B15" s="51" t="s">
+      <c r="A15" s="60"/>
+      <c r="B15" s="67" t="s">
         <v>132</v>
       </c>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="102">
+      <c r="C15" s="68"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="52">
         <f>COUNTA('Inventario No Identificados'!A5:A1048576)</f>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A16" s="103"/>
-      <c r="B16" s="51" t="s">
+      <c r="A16" s="61"/>
+      <c r="B16" s="67" t="s">
         <v>133</v>
       </c>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="53"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="69"/>
       <c r="F16" s="42">
         <f>F3-F4-F15</f>
-        <v>3778</v>
+        <v>3777</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="17.25" customHeight="1">
@@ -1857,50 +2107,50 @@
       <c r="F18" s="43"/>
     </row>
     <row r="19" spans="1:6" s="18" customFormat="1" ht="24">
-      <c r="A19" s="63" t="s">
+      <c r="A19" s="86" t="s">
         <v>134</v>
       </c>
-      <c r="B19" s="64"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="64"/>
-      <c r="E19" s="64"/>
-      <c r="F19" s="65"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="87"/>
+      <c r="D19" s="87"/>
+      <c r="E19" s="87"/>
+      <c r="F19" s="88"/>
     </row>
     <row r="20" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A20" s="104" t="s">
+      <c r="A20" s="89" t="s">
         <v>135</v>
       </c>
-      <c r="B20" s="105"/>
-      <c r="C20" s="105"/>
-      <c r="D20" s="106"/>
-      <c r="E20" s="107" t="s">
+      <c r="B20" s="90"/>
+      <c r="C20" s="90"/>
+      <c r="D20" s="91"/>
+      <c r="E20" s="83" t="s">
         <v>141</v>
       </c>
-      <c r="F20" s="108"/>
+      <c r="F20" s="84"/>
     </row>
     <row r="21" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A21" s="104" t="s">
+      <c r="A21" s="89" t="s">
         <v>136</v>
       </c>
-      <c r="B21" s="105"/>
-      <c r="C21" s="105"/>
-      <c r="D21" s="106"/>
-      <c r="E21" s="107" t="s">
+      <c r="B21" s="90"/>
+      <c r="C21" s="90"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="83" t="s">
         <v>141</v>
       </c>
-      <c r="F21" s="108"/>
+      <c r="F21" s="84"/>
     </row>
     <row r="22" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A22" s="104" t="s">
+      <c r="A22" s="89" t="s">
         <v>137</v>
       </c>
-      <c r="B22" s="105"/>
-      <c r="C22" s="105"/>
-      <c r="D22" s="106"/>
-      <c r="E22" s="109" t="s">
+      <c r="B22" s="90"/>
+      <c r="C22" s="90"/>
+      <c r="D22" s="91"/>
+      <c r="E22" s="85" t="s">
         <v>142</v>
       </c>
-      <c r="F22" s="108"/>
+      <c r="F22" s="84"/>
     </row>
   </sheetData>
   <mergeCells count="25">
@@ -1952,7 +2202,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sheet10">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="B1:G35"/>
@@ -2030,52 +2280,52 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B5" s="79" t="s">
+      <c r="B5" s="105" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="82" t="s">
+      <c r="E5" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="85" t="s">
+      <c r="F5" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="82" t="s">
+      <c r="G5" s="108" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B6" s="80"/>
+      <c r="B6" s="106"/>
       <c r="C6" s="4"/>
       <c r="D6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="83"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="83"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="112"/>
+      <c r="G6" s="109"/>
     </row>
     <row r="7" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B7" s="80"/>
+      <c r="B7" s="106"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="83"/>
-      <c r="F7" s="86"/>
-      <c r="G7" s="83"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="112"/>
+      <c r="G7" s="109"/>
     </row>
     <row r="8" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B8" s="81"/>
+      <c r="B8" s="107"/>
       <c r="C8" s="4"/>
       <c r="D8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="84"/>
-      <c r="F8" s="87"/>
-      <c r="G8" s="84"/>
+      <c r="E8" s="110"/>
+      <c r="F8" s="113"/>
+      <c r="G8" s="110"/>
     </row>
     <row r="9" spans="2:7" ht="17.25" customHeight="1">
       <c r="B9" s="9" t="s">
@@ -2096,32 +2346,32 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B10" s="79" t="s">
+      <c r="B10" s="105" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="82" t="s">
+      <c r="E10" s="108" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="85" t="s">
+      <c r="F10" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="82" t="s">
+      <c r="G10" s="108" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B11" s="81"/>
+      <c r="B11" s="107"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="84"/>
-      <c r="F11" s="87"/>
-      <c r="G11" s="84"/>
+      <c r="E11" s="110"/>
+      <c r="F11" s="113"/>
+      <c r="G11" s="110"/>
     </row>
     <row r="12" spans="2:7" ht="17.25" customHeight="1">
       <c r="B12" s="3" t="s">
@@ -2428,7 +2678,7 @@
       </c>
     </row>
     <row r="30" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B30" s="79" t="s">
+      <c r="B30" s="105" t="s">
         <v>16</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -2437,35 +2687,35 @@
       <c r="D30" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E30" s="82" t="s">
+      <c r="E30" s="108" t="s">
         <v>88</v>
       </c>
-      <c r="F30" s="85" t="s">
+      <c r="F30" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="G30" s="82" t="s">
+      <c r="G30" s="108" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B31" s="80"/>
+      <c r="B31" s="106"/>
       <c r="C31" s="4"/>
       <c r="D31" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E31" s="83"/>
-      <c r="F31" s="86"/>
-      <c r="G31" s="83"/>
+      <c r="E31" s="109"/>
+      <c r="F31" s="112"/>
+      <c r="G31" s="109"/>
     </row>
     <row r="32" spans="2:7" ht="17.25" customHeight="1">
-      <c r="B32" s="81"/>
+      <c r="B32" s="107"/>
       <c r="C32" s="4"/>
       <c r="D32" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E32" s="84"/>
-      <c r="F32" s="87"/>
-      <c r="G32" s="84"/>
+      <c r="E32" s="110"/>
+      <c r="F32" s="113"/>
+      <c r="G32" s="110"/>
     </row>
     <row r="33" spans="2:7" ht="17.25" customHeight="1">
       <c r="B33" s="3" t="s">
@@ -2540,7 +2790,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sheet2">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:G2262"/>
@@ -2568,47 +2818,47 @@
       <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:7" s="18" customFormat="1" ht="24">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="92" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
     </row>
     <row r="4" spans="1:7" s="18" customFormat="1" ht="16" customHeight="1">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="94" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="96" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="96" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="96" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="70" t="s">
+      <c r="E4" s="96" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="70" t="s">
+      <c r="F4" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="70" t="s">
+      <c r="G4" s="96" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="18" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A5" s="69"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
+      <c r="A5" s="95"/>
+      <c r="B5" s="97"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="97"/>
     </row>
     <row r="6" spans="1:7" ht="17.25" customHeight="1">
       <c r="A6" s="19"/>
@@ -13927,7 +14177,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sheet3">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:F5"/>
@@ -13960,14 +14210,14 @@
       <c r="F2" s="17"/>
     </row>
     <row r="3" spans="1:6" s="18" customFormat="1" ht="24">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="92" t="s">
         <v>120</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
     </row>
     <row r="4" spans="1:6" s="18" customFormat="1" ht="17">
       <c r="A4" s="44" t="s">
@@ -14020,7 +14270,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sheet4">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:J6"/>
@@ -14066,64 +14316,64 @@
       <c r="J2" s="17"/>
     </row>
     <row r="3" spans="1:10" s="18" customFormat="1" ht="24">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="92" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="67"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="93"/>
     </row>
     <row r="4" spans="1:10" s="18" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="94" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="96" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="96" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="96" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="70" t="s">
+      <c r="E4" s="96" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="70" t="s">
+      <c r="F4" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="70" t="s">
+      <c r="G4" s="96" t="s">
         <v>115</v>
       </c>
-      <c r="H4" s="72" t="s">
+      <c r="H4" s="98" t="s">
         <v>116</v>
       </c>
-      <c r="I4" s="72"/>
-      <c r="J4" s="70" t="s">
+      <c r="I4" s="98"/>
+      <c r="J4" s="96" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A5" s="69"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
+      <c r="A5" s="95"/>
+      <c r="B5" s="97"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="97"/>
       <c r="H5" s="46" t="s">
         <v>118</v>
       </c>
       <c r="I5" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="J5" s="71"/>
+      <c r="J5" s="97"/>
     </row>
     <row r="6" spans="1:10" ht="18.75" customHeight="1">
       <c r="A6" s="19"/>
@@ -14157,7 +14407,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sheet5">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:K6"/>
@@ -14195,55 +14445,55 @@
       <c r="H2" s="25"/>
     </row>
     <row r="3" spans="1:11" s="18" customFormat="1" ht="24">
-      <c r="A3" s="73" t="s">
+      <c r="A3" s="99" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="73"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="99"/>
       <c r="I3" s="27"/>
       <c r="J3" s="27"/>
       <c r="K3" s="27"/>
     </row>
     <row r="4" spans="1:11" ht="17.25" customHeight="1">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="101" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="102" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="103" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="96" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="70" t="s">
+      <c r="E4" s="96" t="s">
         <v>111</v>
       </c>
-      <c r="F4" s="78" t="s">
+      <c r="F4" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="70" t="s">
+      <c r="G4" s="96" t="s">
         <v>112</v>
       </c>
-      <c r="H4" s="75" t="s">
+      <c r="H4" s="101" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="17.25" customHeight="1">
-      <c r="A5" s="75"/>
-      <c r="B5" s="76"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="75"/>
+      <c r="A5" s="101"/>
+      <c r="B5" s="102"/>
+      <c r="C5" s="103"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="104"/>
+      <c r="G5" s="97"/>
+      <c r="H5" s="101"/>
     </row>
     <row r="6" spans="1:11" ht="17.25" customHeight="1">
       <c r="A6" s="28"/>
@@ -14274,12 +14524,14 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sheet6">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
@@ -14305,29 +14557,29 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:5" s="18" customFormat="1" ht="24">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
     </row>
     <row r="4" spans="1:5" s="18" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A4" s="44" t="s">
-        <v>100</v>
-      </c>
-      <c r="B4" s="45" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="45" t="s">
-        <v>102</v>
-      </c>
-      <c r="D4" s="45" t="s">
-        <v>103</v>
-      </c>
-      <c r="E4" s="45" t="s">
-        <v>104</v>
+      <c r="A4" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="54" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="54" t="s">
+        <v>146</v>
+      </c>
+      <c r="E4" s="55" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17.25" customHeight="1">
@@ -14358,16 +14610,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sheet7">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.5" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" style="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" style="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="23" bestFit="1" customWidth="1"/>
@@ -14389,29 +14643,29 @@
       <c r="E2" s="17"/>
     </row>
     <row r="3" spans="1:5" s="18" customFormat="1" ht="24">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="92" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
     </row>
     <row r="4" spans="1:5" s="18" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A4" s="44" t="s">
-        <v>100</v>
-      </c>
-      <c r="B4" s="45" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="45" t="s">
-        <v>102</v>
-      </c>
-      <c r="D4" s="45" t="s">
-        <v>103</v>
-      </c>
-      <c r="E4" s="45" t="s">
-        <v>104</v>
+      <c r="A4" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="54" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="54" t="s">
+        <v>146</v>
+      </c>
+      <c r="E4" s="55" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17.25" customHeight="1">
@@ -14429,6 +14683,23 @@
       </c>
       <c r="E5" s="21" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16">
+      <c r="A6" s="19">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -14442,30 +14713,102 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sheet8">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="B2:C5"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3">
+      <c r="B2" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sheet9">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="B2:C5"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3">
+      <c r="B2" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New codes with tag
</commit_message>
<xml_diff>
--- a/src/Reporte_Discovery.xlsx
+++ b/src/Reporte_Discovery.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jesusarellano/Documents/TELCEL/AXONIUS/Desarrollo/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D62153-727F-3649-9BBE-0CD394AA4CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD7ADC6-8C07-EF44-9657-435011BC4E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="17120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,8 +35,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="91" r:id="rId11"/>
-    <pivotCache cacheId="92" r:id="rId12"/>
+    <pivotCache cacheId="93" r:id="rId11"/>
+    <pivotCache cacheId="94" r:id="rId12"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1201,6 +1201,39 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1271,39 +1304,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="6" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1501,7 +1501,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B0F87A7E-D022-2E4A-8DDE-C4E01F9C3F96}" name="PivotTable1" cacheId="92" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B0F87A7E-D022-2E4A-8DDE-C4E01F9C3F96}" name="PivotTable1" cacheId="94" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B2:C5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField showAll="0"/>
@@ -1549,7 +1549,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E7C88826-A921-F241-A7D7-09240D889B29}" name="PivotTable2" cacheId="91" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E7C88826-A921-F241-A7D7-09240D889B29}" name="PivotTable2" cacheId="93" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B2:C5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField showAll="0"/>
@@ -1905,80 +1905,80 @@
       <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" s="18" customFormat="1" ht="24">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="58"/>
+      <c r="A2" s="68"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="69"/>
     </row>
     <row r="3" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="89" t="s">
         <v>123</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="80"/>
+      <c r="B3" s="90"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="91"/>
       <c r="F3" s="41">
         <v>7507</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A4" s="59"/>
-      <c r="B4" s="67" t="s">
+      <c r="A4" s="70"/>
+      <c r="B4" s="78" t="s">
         <v>124</v>
       </c>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="69"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="80"/>
       <c r="F4" s="42">
         <f>F5+F10+F13+F14</f>
         <v>3729</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A5" s="60"/>
-      <c r="B5" s="62"/>
-      <c r="C5" s="73" t="s">
+      <c r="A5" s="71"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="84" t="s">
         <v>125</v>
       </c>
-      <c r="D5" s="74"/>
-      <c r="E5" s="75"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="86"/>
       <c r="F5" s="47">
         <f>COUNTA(Inventario!B6:B1048576)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A6" s="60"/>
-      <c r="B6" s="63"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="81" t="s">
+      <c r="A6" s="71"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="57" t="s">
         <v>126</v>
       </c>
-      <c r="E6" s="82"/>
+      <c r="E6" s="58"/>
       <c r="F6" s="48">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A7" s="60"/>
-      <c r="B7" s="63"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="81" t="s">
+      <c r="A7" s="71"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="E7" s="82"/>
+      <c r="E7" s="58"/>
       <c r="F7" s="48">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A8" s="60"/>
-      <c r="B8" s="63"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="62"/>
+      <c r="A8" s="71"/>
+      <c r="B8" s="74"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="73"/>
       <c r="E8" s="49" t="s">
         <v>139</v>
       </c>
@@ -1988,10 +1988,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A9" s="60"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="64"/>
+      <c r="A9" s="71"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="75"/>
       <c r="E9" s="49" t="s">
         <v>140</v>
       </c>
@@ -2001,90 +2001,90 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A10" s="60"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="73" t="s">
+      <c r="A10" s="71"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="84" t="s">
         <v>127</v>
       </c>
-      <c r="D10" s="74"/>
-      <c r="E10" s="75"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="86"/>
       <c r="F10" s="47">
         <f>COUNTA('Inventario - PC'!B6:B1048576)</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A11" s="60"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="76" t="s">
+      <c r="A11" s="71"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="87" t="s">
         <v>128</v>
       </c>
-      <c r="E11" s="77"/>
+      <c r="E11" s="88"/>
       <c r="F11" s="50">
         <f>COUNTIF('Inventario - PC'!F6:F1048576,"SI")</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A12" s="60"/>
-      <c r="B12" s="63"/>
-      <c r="C12" s="66"/>
-      <c r="D12" s="76" t="s">
+      <c r="A12" s="71"/>
+      <c r="B12" s="74"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="87" t="s">
         <v>129</v>
       </c>
-      <c r="E12" s="77"/>
+      <c r="E12" s="88"/>
       <c r="F12" s="50">
         <f>COUNTIF('Inventario - PC'!F6:F1048576,"no")</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A13" s="60"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="73" t="s">
+      <c r="A13" s="71"/>
+      <c r="B13" s="74"/>
+      <c r="C13" s="84" t="s">
         <v>130</v>
       </c>
-      <c r="D13" s="74"/>
-      <c r="E13" s="75"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="86"/>
       <c r="F13" s="47">
         <v>3726</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A14" s="60"/>
-      <c r="B14" s="64"/>
-      <c r="C14" s="73" t="s">
+      <c r="A14" s="71"/>
+      <c r="B14" s="75"/>
+      <c r="C14" s="84" t="s">
         <v>131</v>
       </c>
-      <c r="D14" s="74"/>
-      <c r="E14" s="75"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="86"/>
       <c r="F14" s="47">
         <f>COUNTA('Inventario Identificados'!A5:A1048576)</f>
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A15" s="60"/>
-      <c r="B15" s="67" t="s">
+      <c r="A15" s="71"/>
+      <c r="B15" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="C15" s="68"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="69"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="80"/>
       <c r="F15" s="52">
         <f>COUNTA('Inventario No Identificados'!A5:A1048576)</f>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A16" s="61"/>
-      <c r="B16" s="67" t="s">
+      <c r="A16" s="72"/>
+      <c r="B16" s="78" t="s">
         <v>133</v>
       </c>
-      <c r="C16" s="68"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="69"/>
+      <c r="C16" s="79"/>
+      <c r="D16" s="79"/>
+      <c r="E16" s="80"/>
       <c r="F16" s="42">
         <f>F3-F4-F15</f>
         <v>3777</v>
@@ -2107,62 +2107,53 @@
       <c r="F18" s="43"/>
     </row>
     <row r="19" spans="1:6" s="18" customFormat="1" ht="24">
-      <c r="A19" s="86" t="s">
+      <c r="A19" s="62" t="s">
         <v>134</v>
       </c>
-      <c r="B19" s="87"/>
-      <c r="C19" s="87"/>
-      <c r="D19" s="87"/>
-      <c r="E19" s="87"/>
-      <c r="F19" s="88"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="64"/>
     </row>
     <row r="20" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A20" s="89" t="s">
+      <c r="A20" s="65" t="s">
         <v>135</v>
       </c>
-      <c r="B20" s="90"/>
-      <c r="C20" s="90"/>
-      <c r="D20" s="91"/>
-      <c r="E20" s="83" t="s">
+      <c r="B20" s="66"/>
+      <c r="C20" s="66"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="59" t="s">
         <v>141</v>
       </c>
-      <c r="F20" s="84"/>
+      <c r="F20" s="60"/>
     </row>
     <row r="21" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A21" s="89" t="s">
+      <c r="A21" s="65" t="s">
         <v>136</v>
       </c>
-      <c r="B21" s="90"/>
-      <c r="C21" s="90"/>
-      <c r="D21" s="91"/>
-      <c r="E21" s="83" t="s">
+      <c r="B21" s="66"/>
+      <c r="C21" s="66"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="59" t="s">
         <v>141</v>
       </c>
-      <c r="F21" s="84"/>
+      <c r="F21" s="60"/>
     </row>
     <row r="22" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A22" s="89" t="s">
+      <c r="A22" s="65" t="s">
         <v>137</v>
       </c>
-      <c r="B22" s="90"/>
-      <c r="C22" s="90"/>
-      <c r="D22" s="91"/>
-      <c r="E22" s="85" t="s">
+      <c r="B22" s="66"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="61" t="s">
         <v>142</v>
       </c>
-      <c r="F22" s="84"/>
+      <c r="F22" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A22:D22"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A4:A16"/>
     <mergeCell ref="B5:B14"/>
@@ -2179,6 +2170,15 @@
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="C5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A22:D22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F5" location="Inventario!A1" display="Inventario!A1" xr:uid="{B80F5769-9041-D946-A663-3C05C393B9EF}"/>

</xml_diff>